<commit_message>
Correcion primer puesto coquina
</commit_message>
<xml_diff>
--- a/data/clasf_jor10_gB.xlsx
+++ b/data/clasf_jor10_gB.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28318"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DB1DB4D8-D3AD-4AAF-842F-015372381F84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1B173E72-1658-4C12-8BE1-9027D7030937}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -438,7 +438,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -503,7 +503,7 @@
         <v>16</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3">
         <v>67</v>

</xml_diff>